<commit_message>
XLSX & CSV Import/export tests
</commit_message>
<xml_diff>
--- a/backend/debug/data/import.xlsx
+++ b/backend/debug/data/import.xlsx
@@ -1,45 +1,78 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2">
+  <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookProtection/>
+  <bookViews>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
-  <si>
-    <t>Field 1</t>
-  </si>
-  <si>
-    <t>Field 2</t>
-  </si>
-  <si>
-    <t>c1</t>
-  </si>
-  <si>
-    <t>c2</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
+  <si>
+    <t xml:space="preserve">Field 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Field 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">egg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
-    <font>
-      <sz val="10.0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="General"/>
+  </numFmts>
+  <fonts count="5">
+    <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
-      <scheme val="minor"/>
+      <family val="0"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -47,32 +80,62 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+  <cellStyleXfs count="20">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+  <cellStyles count="6">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -83,94 +146,90 @@
         <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="FFFFFF"/>
+        <a:srgbClr val="ffffff"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="000000"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="FFFFFF"/>
+        <a:srgbClr val="ffffff"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4285F4"/>
+        <a:srgbClr val="4285f4"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="EA4335"/>
+        <a:srgbClr val="ea4335"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="FBBC04"/>
+        <a:srgbClr val="fbbc04"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="34A853"/>
+        <a:srgbClr val="34a853"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="FF6D01"/>
+        <a:srgbClr val="ff6d01"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="46BDC6"/>
+        <a:srgbClr val="46bdc6"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="1155CC"/>
+        <a:srgbClr val="1155cc"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="1155CC"/>
+        <a:srgbClr val="1155cc"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Sheets">
       <a:majorFont>
-        <a:latin typeface="Arial"/>
-        <a:ea typeface="Arial"/>
-        <a:cs typeface="Arial"/>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:cs typeface="Arial" pitchFamily="0" charset="1"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Arial"/>
-        <a:ea typeface="Arial"/>
-        <a:cs typeface="Arial"/>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:cs typeface="Arial" pitchFamily="0" charset="1"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme>
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
                 <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
                 <a:tint val="67000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="50000">
               <a:schemeClr val="phClr">
                 <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
                 <a:tint val="73000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
                 <a:tint val="81000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
         </a:gradFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
                 <a:lumMod val="102000"/>
                 <a:tint val="94000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
                 <a:lumMod val="100000"/>
                 <a:shade val="100000"/>
               </a:schemeClr>
@@ -178,33 +237,24 @@
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
                 <a:shade val="78000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
         <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
@@ -217,13 +267,7 @@
           <a:effectLst/>
         </a:effectStyle>
         <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
+          <a:effectLst/>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
@@ -233,15 +277,13 @@
         <a:solidFill>
           <a:schemeClr val="phClr">
             <a:tint val="95000"/>
-            <a:satMod val="170000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
                 <a:tint val="93000"/>
-                <a:satMod val="150000"/>
                 <a:shade val="98000"/>
                 <a:lumMod val="102000"/>
               </a:schemeClr>
@@ -249,7 +291,6 @@
             <a:gs pos="50000">
               <a:schemeClr val="phClr">
                 <a:tint val="98000"/>
-                <a:satMod val="130000"/>
                 <a:shade val="90000"/>
                 <a:lumMod val="103000"/>
               </a:schemeClr>
@@ -257,11 +298,11 @@
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:shade val="63000"/>
-                <a:satMod val="120000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
@@ -270,16 +311,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <outlinePr summaryBelow="0"/>
+    <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1">
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -287,39 +332,45 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="3">
+      <c r="B2" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="4">
+      <c r="B3" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="1">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="5">
+      <c r="B4" s="1" t="n">
+        <v>3.65151</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="1">
-        <v>5.0</v>
+      <c r="B5" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>